<commit_message>
product technical details inserted in database
</commit_message>
<xml_diff>
--- a/src/app/data_to_dict.xlsx
+++ b/src/app/data_to_dict.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>Key</t>
   </si>
@@ -21,125 +21,164 @@
     <t>Value</t>
   </si>
   <si>
-    <t>OS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">‎MIUI 12.5 based on Android 11</t>
-  </si>
-  <si>
-    <t>RAM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">‎6 GB</t>
+    <t>Cuisine</t>
+  </si>
+  <si>
+    <t>‎Indian</t>
+  </si>
+  <si>
+    <t>Specialty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">‎Preservatives Free, Vegetarian, Artificial Flavor Free</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">‎910 Grams</t>
+  </si>
+  <si>
+    <t>Volume</t>
+  </si>
+  <si>
+    <t xml:space="preserve">‎1 Litres</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ingredient Type</t>
+  </si>
+  <si>
+    <t>‎Vegetarian</t>
+  </si>
+  <si>
+    <t>Brand</t>
+  </si>
+  <si>
+    <t>‎FIGARO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Storage Instructions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">‎Store tightly capped in a cold dry place, away from light.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Item Package Quantity</t>
+  </si>
+  <si>
+    <t>‎1</t>
+  </si>
+  <si>
+    <t>Form</t>
+  </si>
+  <si>
+    <t>‎Fresh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Appropriate Age Range</t>
+  </si>
+  <si>
+    <t xml:space="preserve">‎36 Months</t>
+  </si>
+  <si>
+    <t>Taste</t>
+  </si>
+  <si>
+    <t>‎Mild</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Serving Recommendation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">‎Please serve it at room temperature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Package Information</t>
+  </si>
+  <si>
+    <t>‎Bottle</t>
+  </si>
+  <si>
+    <t>‎Jar</t>
+  </si>
+  <si>
+    <t>Manufacturer</t>
+  </si>
+  <si>
+    <t>‎Figaro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Item model number</t>
+  </si>
+  <si>
+    <t>‎8410125609477</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Net Quantity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">‎1000.0 millilitre</t>
   </si>
   <si>
     <t xml:space="preserve">Product Dimensions</t>
   </si>
   <si>
-    <t xml:space="preserve">‎16.4 x 0.9 x 7.6 cm; 195 Grams</t>
-  </si>
-  <si>
-    <t>Batteries</t>
-  </si>
-  <si>
-    <t xml:space="preserve">‎1 Lithium Polymer batteries required. (included)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Item model number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">‎Redmi Note 11T 5G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Connectivity technologies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">‎WiFi Bluetooth;Infrared;Wi-Fi;USB</t>
-  </si>
-  <si>
-    <t>GPS</t>
-  </si>
-  <si>
-    <t>‎True</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Special features</t>
-  </si>
-  <si>
-    <t xml:space="preserve">‎3.5mm Jack, IR Blaster, X-Axis Linear Vibration Motor, Corning gorilla glass 3 protection, Dual Stereo Speakers for immersive audio experience. Hi-Res certified audio, Splash, Water and Dust Resistant- IP53</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other display features</t>
-  </si>
-  <si>
-    <t>‎Wireless</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Device interface - primary</t>
-  </si>
-  <si>
-    <t>‎Touchscreen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other camera features</t>
-  </si>
-  <si>
-    <t>‎Front</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Audio Jack</t>
-  </si>
-  <si>
-    <t xml:space="preserve">‎3.5 mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Form factor</t>
-  </si>
-  <si>
-    <t>‎Phablet</t>
-  </si>
-  <si>
-    <t>Colour</t>
-  </si>
-  <si>
-    <t xml:space="preserve">‎Aquamarine Blue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Battery Power Rating</t>
-  </si>
-  <si>
-    <t>‎5000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Whats in the box</t>
-  </si>
-  <si>
-    <t xml:space="preserve">‎Redmi Note 11T 5G, Power adapter, USB cable, SIM eject tool, Warranty card, User guide, Clear soft case, Screen protector pre-applied on the phone</t>
-  </si>
-  <si>
-    <t>Manufacturer</t>
-  </si>
-  <si>
-    <t>‎Redmi</t>
+    <t xml:space="preserve">‎9.5 x 7 x 18.5 cm; 910 Grams</t>
+  </si>
+  <si>
+    <t>Ingredients</t>
+  </si>
+  <si>
+    <t xml:space="preserve">‎Olive Oil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Serving Size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">‎14 Grams</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energy (kcal)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">‎30.11 Kilocalories</t>
+  </si>
+  <si>
+    <t>Protein</t>
+  </si>
+  <si>
+    <t xml:space="preserve">‎0 Grams</t>
+  </si>
+  <si>
+    <t>Fat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">‎14.00 Grams</t>
+  </si>
+  <si>
+    <t>Carbohydrate</t>
+  </si>
+  <si>
+    <t>Sodium</t>
   </si>
   <si>
     <t xml:space="preserve">Country of Origin</t>
   </si>
   <si>
-    <t>‎India</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Item Weight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">‎195 g</t>
+    <t>‎Spain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Imported By</t>
+  </si>
+  <si>
+    <t xml:space="preserve">‎Deoleo India Pvt Mtd</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <color theme="1"/>
@@ -148,16 +187,27 @@
     </font>
     <font>
       <name val="Liberation Sans"/>
+      <color rgb="FF0F1111"/>
+      <sz val="10.500000"/>
+    </font>
+    <font>
+      <name val="Liberation Sans"/>
       <color indexed="63"/>
       <sz val="10.500000"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF3F3F3"/>
+        <bgColor rgb="FFF3F3F3"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -181,9 +231,12 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="1" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf fontId="2" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -693,14 +746,14 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="32.421875"/>
-    <col customWidth="1" min="2" max="2" width="41.28125"/>
+    <col customWidth="1" min="1" max="1" width="19.28125"/>
+    <col customWidth="1" min="2" max="2" width="28.8515625"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
@@ -711,166 +764,222 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" ht="14.25">
-      <c r="A2" t="s">
+    <row r="2" ht="255">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" ht="255">
-      <c r="A3" t="s">
+    <row r="3" ht="38.25">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" ht="14.25">
-      <c r="A4" t="s">
+    <row r="4" ht="25.5">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" ht="25.5">
-      <c r="A5" t="s">
+    <row r="5" ht="14.25">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" ht="14.25">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" ht="14.25">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" ht="14.25">
-      <c r="A8" t="s">
+    <row r="8" ht="76.5">
+      <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" ht="76.5">
-      <c r="A9" t="s">
+    <row r="9" ht="25.5">
+      <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" ht="14.25">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" ht="14.25">
-      <c r="A11" t="s">
+    <row r="11" ht="25.5">
+      <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" ht="25.5">
-      <c r="A12" t="s">
+    <row r="12" ht="14.25">
+      <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="13" ht="25.5">
-      <c r="A13" t="s">
+      <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="14" ht="25.5">
-      <c r="A14" t="s">
+      <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" ht="14.25">
-      <c r="A15" t="s">
+    <row r="15" ht="25.5">
+      <c r="A15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="1" t="s">
+    </row>
+    <row r="16" ht="14.25">
+      <c r="A16" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="16" ht="14.25">
-      <c r="A16" t="s">
+      <c r="B16" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="1" t="s">
+    </row>
+    <row r="17" ht="14.25">
+      <c r="A17" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="17" ht="51">
-      <c r="A17" t="s">
+      <c r="B17" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="1" t="s">
+    </row>
+    <row r="18" ht="25.5">
+      <c r="A18" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="18" ht="14.25">
-      <c r="A18" t="s">
+      <c r="B18" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="1" t="s">
+    </row>
+    <row r="19" ht="14.25">
+      <c r="A19" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="19" ht="25.5">
-      <c r="A19" t="s">
+      <c r="B19" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="1" t="s">
+    </row>
+    <row r="20" ht="14.25">
+      <c r="A20" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="20" ht="14.25">
-      <c r="A20" t="s">
+      <c r="B20" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="1" t="s">
+    </row>
+    <row r="21" ht="14.25">
+      <c r="A21" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="21" ht="14.25"/>
-    <row r="22" ht="14.25"/>
-    <row r="23" ht="14.25"/>
-    <row r="24" ht="14.25"/>
-    <row r="25" ht="14.25"/>
-    <row r="26" ht="14.25"/>
-    <row r="27" ht="14.25"/>
-    <row r="28" ht="14.25"/>
+      <c r="B21" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" ht="14.25">
+      <c r="A22" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" ht="14.25">
+      <c r="A23" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" ht="14.25">
+      <c r="A24" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" ht="14.25">
+      <c r="A25" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" ht="14.25">
+      <c r="A26" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" ht="14.25">
+      <c r="A27" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" ht="14.25">
+      <c r="A28" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
     <row r="29" ht="14.25"/>
     <row r="30" ht="14.25"/>
     <row r="31" ht="14.25"/>
@@ -881,34 +990,12 @@
     <row r="36" ht="14.25"/>
     <row r="37" ht="14.25"/>
     <row r="38" ht="14.25"/>
-    <row r="39" ht="25.5"/>
+    <row r="39" ht="14.25"/>
     <row r="40" ht="14.25"/>
-    <row r="41" ht="14.25"/>
-    <row r="42" ht="14.25"/>
-    <row r="43" ht="14.25"/>
-    <row r="44" ht="14.25"/>
-    <row r="45" ht="14.25"/>
-    <row r="46" ht="14.25"/>
-    <row r="47" ht="14.25"/>
-    <row r="48" ht="14.25"/>
-    <row r="49" ht="14.25"/>
-    <row r="50" ht="14.25"/>
-    <row r="51" ht="14.25"/>
-    <row r="52" ht="14.25"/>
-    <row r="53" ht="14.25"/>
-    <row r="54" ht="14.25"/>
-    <row r="55" ht="14.25"/>
-    <row r="56" ht="14.25"/>
-    <row r="57" ht="14.25"/>
-    <row r="58" ht="14.25"/>
-    <row r="59" ht="14.25"/>
-    <row r="60" ht="14.25"/>
-    <row r="61" ht="14.25"/>
-    <row r="62" ht="14.25"/>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="4294967295" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="2147483648" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>